<commit_message>
Move tests to English
</commit_message>
<xml_diff>
--- a/tests/data/base_listing.xlsx
+++ b/tests/data/base_listing.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
-    <t xml:space="preserve">Prénom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courriel</t>
+    <t xml:space="preserve">First name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
   </si>
   <si>
     <t xml:space="preserve">Cours</t>
@@ -367,7 +367,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Check for and fix warnings
</commit_message>
<xml_diff>
--- a/tests/data/base_listing.xlsx
+++ b/tests/data/base_listing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Tutorial</t>
   </si>
   <si>
+    <t xml:space="preserve">Practical work</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
+    <t xml:space="preserve">PW1</t>
+  </si>
+  <si>
     <t xml:space="preserve">blablahm</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t xml:space="preserve">pierre.blahblahfoo@etu.utc.fr</t>
   </si>
   <si>
+    <t xml:space="preserve">PW2</t>
+  </si>
+  <si>
     <t xml:space="preserve">pblahbla</t>
   </si>
   <si>
@@ -82,6 +91,9 @@
     <t xml:space="preserve">D2</t>
   </si>
   <si>
+    <t xml:space="preserve">PW3</t>
+  </si>
+  <si>
     <t xml:space="preserve">mabarbar</t>
   </si>
   <si>
@@ -89,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">mathilde.barbarbar@etu.utc.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PW4</t>
   </si>
   <si>
     <t xml:space="preserve">cblahfoo</t>
@@ -364,10 +379,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,165 +409,192 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>